<commit_message>
updated data_dictionary and added new data file
</commit_message>
<xml_diff>
--- a/documents/data_dictionary.xlsx
+++ b/documents/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmois\Documents\GitHub\RCC-Recurrence-Predictor\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE22304-1F58-4B24-B454-E75C680911F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FADD99-ACB2-4914-9A95-C08C741BB5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{4B67CEAD-0EB3-460C-89B7-16B677CADF4D}"/>
+    <workbookView xWindow="495" yWindow="1230" windowWidth="11445" windowHeight="9000" xr2:uid="{4B67CEAD-0EB3-460C-89B7-16B677CADF4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,155 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>yos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age </t>
+  </si>
+  <si>
+    <t>year of surgery</t>
+  </si>
+  <si>
+    <t>Cytoreductive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whether or not the procedure was cytoreductive </t>
+  </si>
+  <si>
+    <t>readmin30</t>
+  </si>
+  <si>
+    <t>readmission before 30 days</t>
+  </si>
+  <si>
+    <t>comorbid0</t>
+  </si>
+  <si>
+    <t>Comorbidites Equal to 0</t>
+  </si>
+  <si>
+    <t>comorbid1</t>
+  </si>
+  <si>
+    <t>Comorbidities Equal to 1</t>
+  </si>
+  <si>
+    <t>comorbid2</t>
+  </si>
+  <si>
+    <t>Comorbidities Equal to 2</t>
+  </si>
+  <si>
+    <t>comorbid3_plus</t>
+  </si>
+  <si>
+    <t>Comorbidities &gt;= 3</t>
+  </si>
+  <si>
+    <t>lap</t>
+  </si>
+  <si>
+    <t>Laproscopic</t>
+  </si>
+  <si>
+    <t>robot</t>
+  </si>
+  <si>
+    <t>Robotic</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Open Surgery</t>
+  </si>
+  <si>
+    <t>ebl</t>
+  </si>
+  <si>
+    <t>EBL</t>
+  </si>
+  <si>
+    <t>Readmission within 30 days</t>
+  </si>
+  <si>
+    <t>padua</t>
+  </si>
+  <si>
+    <t>Padua Score</t>
+  </si>
+  <si>
+    <t>renal</t>
+  </si>
+  <si>
+    <t>Renal Score</t>
+  </si>
+  <si>
+    <t>bmi</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>recurrence</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>r_depth</t>
+  </si>
+  <si>
+    <t>r_location</t>
+  </si>
+  <si>
+    <t>r_laterality</t>
+  </si>
+  <si>
+    <t>r_invasion</t>
+  </si>
+  <si>
+    <t>resection depth</t>
+  </si>
+  <si>
+    <t>kideny region</t>
+  </si>
+  <si>
+    <t>level vascular invasion</t>
+  </si>
+  <si>
+    <t>procedure laterality</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +206,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,14 +529,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB577C1-A92D-4851-A843-ED85A79ECDED}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>